<commit_message>
Update Chapter 4 examples with steelP.mod and steelP.dat example.
</commit_message>
<xml_diff>
--- a/AMPL_Book_Examples_Chp4.xlsx
+++ b/AMPL_Book_Examples_Chp4.xlsx
@@ -4,12 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15315" windowHeight="12345"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15315" windowHeight="12345" tabRatio="524" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="multi" sheetId="4" r:id="rId1"/>
+    <sheet name="steelT" sheetId="7" r:id="rId2"/>
+    <sheet name="steelP" sheetId="9" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="avail" localSheetId="2">steelP!$B$7:$D$7</definedName>
+    <definedName name="avail" localSheetId="1">steelT!$B$10:$E$10</definedName>
+    <definedName name="avail.badindex" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="avail.badindex" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="avail.columnindex" localSheetId="2" hidden="1">steelP!$B$6:$D$6</definedName>
+    <definedName name="avail.columnindex" localSheetId="1" hidden="1">steelT!$B$9:$E$9</definedName>
+    <definedName name="avail.columnindex.dirn" localSheetId="2" hidden="1">"column"</definedName>
+    <definedName name="avail.columnindex.dirn" localSheetId="1" hidden="1">"column"</definedName>
     <definedName name="cost_bands" localSheetId="0">multi!$C$17:$I$19</definedName>
     <definedName name="cost_bands.badindex" localSheetId="0" hidden="1">1</definedName>
     <definedName name="cost_bands.columnindex" localSheetId="0" hidden="1">multi!$C$16:$I$16</definedName>
@@ -32,21 +42,110 @@
     <definedName name="cost_plate.rowindex" localSheetId="0" hidden="1">multi!$B$23:$B$25</definedName>
     <definedName name="cost_plate.rowindex.dirn" localSheetId="0" hidden="1">"row"</definedName>
     <definedName name="demand" localSheetId="0">multi!$C$12:$I$14</definedName>
+    <definedName name="demand" localSheetId="2">steelP!$B$18:$H$20</definedName>
     <definedName name="demand.badindex" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="demand.badindex" localSheetId="2" hidden="1">1</definedName>
     <definedName name="demand.columnindex" localSheetId="0" hidden="1">multi!$C$11:$I$11</definedName>
+    <definedName name="demand.columnindex" localSheetId="2" hidden="1">steelP!$B$17:$H$17</definedName>
     <definedName name="demand.columnindex.dirn" localSheetId="0" hidden="1">"column"</definedName>
+    <definedName name="demand.columnindex.dirn" localSheetId="2" hidden="1">"column"</definedName>
     <definedName name="demand.firstindex" localSheetId="0" hidden="1">"column"</definedName>
+    <definedName name="demand.firstindex" localSheetId="2" hidden="1">"column"</definedName>
     <definedName name="demand.rowindex" localSheetId="0" hidden="1">multi!$B$12:$B$14</definedName>
+    <definedName name="demand.rowindex" localSheetId="2" hidden="1">steelP!$A$18:$A$20</definedName>
     <definedName name="demand.rowindex.dirn" localSheetId="0" hidden="1">"row"</definedName>
+    <definedName name="demand.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
     <definedName name="demandcolumnindex.dirn" localSheetId="0">"Column"</definedName>
     <definedName name="demandrowindex.dirn" localSheetId="0">"Row"</definedName>
     <definedName name="DEST" localSheetId="0">multi!$C$3:$I$3</definedName>
+    <definedName name="DEST" localSheetId="2">steelP!$B$3:$H$3</definedName>
     <definedName name="DEST.dirn" localSheetId="0" hidden="1">"column"</definedName>
+    <definedName name="DEST.dirn" localSheetId="2" hidden="1">"column"</definedName>
+    <definedName name="Inv" localSheetId="1">steelT!$B$23:$F$24</definedName>
+    <definedName name="Inv.badindex" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="Inv.columnindex" localSheetId="1" hidden="1">steelT!$B$22:$F$22</definedName>
+    <definedName name="Inv.columnindex.dirn" localSheetId="1" hidden="1">"column"</definedName>
+    <definedName name="Inv.firstindex" localSheetId="1" hidden="1">"row"</definedName>
+    <definedName name="Inv.rowindex" localSheetId="1" hidden="1">steelT!$A$23:$A$24</definedName>
+    <definedName name="Inv.rowindex.dirn" localSheetId="1" hidden="1">"row"</definedName>
+    <definedName name="inv0" localSheetId="1">steelT!$B$4:$C$4</definedName>
+    <definedName name="inv0.badindex" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="inv0.columnindex" localSheetId="1" hidden="1">steelT!$B$2:$C$2</definedName>
+    <definedName name="inv0.columnindex.dirn" localSheetId="1" hidden="1">"column"</definedName>
+    <definedName name="invcost" localSheetId="1">steelT!$B$6:$C$6</definedName>
+    <definedName name="invcost.badindex" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="invcost.columnindex" localSheetId="1" hidden="1">steelT!$B$2:$C$2</definedName>
+    <definedName name="invcost.columnindex.dirn" localSheetId="1" hidden="1">"column"</definedName>
+    <definedName name="Make" localSheetId="2">steelP!$B$48:$D$50</definedName>
+    <definedName name="Make" localSheetId="1">steelT!$C$20:$F$21</definedName>
+    <definedName name="Make.badindex" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="Make.badindex" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="Make.columnindex" localSheetId="2" hidden="1">steelP!$B$47:$D$47</definedName>
+    <definedName name="Make.columnindex" localSheetId="1" hidden="1">steelT!$C$19:$F$19</definedName>
+    <definedName name="Make.columnindex.dirn" localSheetId="2" hidden="1">"column"</definedName>
+    <definedName name="Make.columnindex.dirn" localSheetId="1" hidden="1">"column"</definedName>
+    <definedName name="Make.firstindex" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="Make.firstindex" localSheetId="1" hidden="1">"row"</definedName>
+    <definedName name="Make.rowindex" localSheetId="2" hidden="1">steelP!$A$48:$A$50</definedName>
+    <definedName name="Make.rowindex" localSheetId="1" hidden="1">steelT!$A$20:$A$21</definedName>
+    <definedName name="Make.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="Make.rowindex.dirn" localSheetId="1" hidden="1">"row"</definedName>
+    <definedName name="make_cost" localSheetId="2">steelP!$B$13:$D$15</definedName>
+    <definedName name="make_cost.badindex" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="make_cost.columnindex" localSheetId="2" hidden="1">steelP!$B$12:$D$12</definedName>
+    <definedName name="make_cost.columnindex.dirn" localSheetId="2" hidden="1">"column"</definedName>
+    <definedName name="make_cost.firstindex" localSheetId="2" hidden="1">"column"</definedName>
+    <definedName name="make_cost.rowindex" localSheetId="2" hidden="1">steelP!$A$13:$A$15</definedName>
+    <definedName name="make_cost.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="market" localSheetId="1">steelT!$B$16:$E$17</definedName>
+    <definedName name="market.badindex" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="market.columnindex" localSheetId="1" hidden="1">steelT!$B$15:$E$15</definedName>
+    <definedName name="market.columnindex.dirn" localSheetId="1" hidden="1">"column"</definedName>
+    <definedName name="market.firstindex" localSheetId="1" hidden="1">"row"</definedName>
+    <definedName name="market.rowindex" localSheetId="1" hidden="1">steelT!$A$16:$A$17</definedName>
+    <definedName name="market.rowindex.dirn" localSheetId="1" hidden="1">"row"</definedName>
     <definedName name="ORIG" localSheetId="0">multi!$C$2:$E$2</definedName>
+    <definedName name="ORIG" localSheetId="2">steelP!$B$2:$D$2</definedName>
     <definedName name="ORIG.dirn" localSheetId="0" hidden="1">"column"</definedName>
+    <definedName name="ORIG.dirn" localSheetId="2" hidden="1">"column"</definedName>
     <definedName name="PROD" localSheetId="0">multi!$C$4:$E$4</definedName>
+    <definedName name="PROD" localSheetId="2">steelP!$B$4:$D$4</definedName>
+    <definedName name="PROD" localSheetId="1">steelT!$B$2:$C$2</definedName>
     <definedName name="PROD.dirn" localSheetId="0" hidden="1">"column"</definedName>
+    <definedName name="PROD.dirn" localSheetId="2" hidden="1">"column"</definedName>
+    <definedName name="PROD.dirn" localSheetId="1" hidden="1">"column"</definedName>
+    <definedName name="prodcost" localSheetId="1">steelT!$B$5:$C$5</definedName>
+    <definedName name="prodcost.badindex" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="prodcost.columnindex" localSheetId="1" hidden="1">steelT!$B$2:$C$2</definedName>
+    <definedName name="prodcost.columnindex.dirn" localSheetId="1" hidden="1">"column"</definedName>
+    <definedName name="rate" localSheetId="2">steelP!$B$9:$D$11</definedName>
+    <definedName name="rate" localSheetId="1">steelT!$B$3:$C$3</definedName>
+    <definedName name="rate.badindex" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="rate.badindex" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="rate.columnindex" localSheetId="2" hidden="1">steelP!$B$6:$D$6</definedName>
+    <definedName name="rate.columnindex" localSheetId="1" hidden="1">steelT!$B$2:$C$2</definedName>
+    <definedName name="rate.columnindex.dirn" localSheetId="2" hidden="1">"column"</definedName>
+    <definedName name="rate.columnindex.dirn" localSheetId="1" hidden="1">"column"</definedName>
+    <definedName name="rate.firstindex" localSheetId="2" hidden="1">"column"</definedName>
+    <definedName name="rate.rowindex" localSheetId="2" hidden="1">steelP!$A$9:$A$11</definedName>
+    <definedName name="rate.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="revenue" localSheetId="1">steelT!$B$13:$E$14</definedName>
+    <definedName name="revenue.badindex" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="revenue.columnindex" localSheetId="1" hidden="1">steelT!$B$12:$E$12</definedName>
+    <definedName name="revenue.columnindex.dirn" localSheetId="1" hidden="1">"column"</definedName>
+    <definedName name="revenue.firstindex" localSheetId="1" hidden="1">"row"</definedName>
+    <definedName name="revenue.rowindex" localSheetId="1" hidden="1">steelT!$A$13:$A$14</definedName>
+    <definedName name="revenue.rowindex.dirn" localSheetId="1" hidden="1">"row"</definedName>
+    <definedName name="Sell" localSheetId="1">steelT!$C$26:$F$27</definedName>
+    <definedName name="Sell.badindex" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="Sell.columnindex" localSheetId="1" hidden="1">steelT!$C$25:$F$25</definedName>
+    <definedName name="Sell.columnindex.dirn" localSheetId="1" hidden="1">"column"</definedName>
+    <definedName name="Sell.firstindex" localSheetId="1" hidden="1">"row"</definedName>
+    <definedName name="Sell.rowindex" localSheetId="1" hidden="1">steelT!$A$26:$A$27</definedName>
+    <definedName name="Sell.rowindex.dirn" localSheetId="1" hidden="1">"row"</definedName>
     <definedName name="solve_result" localSheetId="0">multi!$A$39</definedName>
+    <definedName name="solve_result" localSheetId="2">steelP!$A$56</definedName>
+    <definedName name="solve_result" localSheetId="1">steelT!$A$30</definedName>
     <definedName name="supply" localSheetId="0">multi!$C$7:$E$9</definedName>
     <definedName name="supply.badindex" localSheetId="0" hidden="1">1</definedName>
     <definedName name="supply.columnindex" localSheetId="0" hidden="1">multi!$C$6:$E$6</definedName>
@@ -56,35 +155,84 @@
     <definedName name="supply.rowindex.dirn" localSheetId="0" hidden="1">"row"</definedName>
     <definedName name="supplycolumnindex.dirn" localSheetId="0">"Column"</definedName>
     <definedName name="supplyrowindex.dirn" localSheetId="0">"Row"</definedName>
+    <definedName name="T" localSheetId="1">steelT!$B$8</definedName>
+    <definedName name="Time" localSheetId="2">steelP!$B$53:$D$53</definedName>
+    <definedName name="Time.badindex" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="Time.columnindex" localSheetId="2" hidden="1">steelP!$B$52:$D$52</definedName>
+    <definedName name="Time.columnindex.dirn" localSheetId="2" hidden="1">"column"</definedName>
     <definedName name="Total_Cost" localSheetId="0">multi!$D$39</definedName>
+    <definedName name="Total_Cost" localSheetId="2">steelP!$D$56</definedName>
+    <definedName name="total_profit" localSheetId="1">steelT!$D$30</definedName>
     <definedName name="Trans_bands" localSheetId="0">multi!$C$28:$I$30</definedName>
+    <definedName name="Trans_bands" localSheetId="2">steelP!$B$35:$H$37</definedName>
     <definedName name="Trans_bands.badindex" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="Trans_bands.badindex" localSheetId="2" hidden="1">1</definedName>
     <definedName name="Trans_bands.columnindex" localSheetId="0" hidden="1">multi!$C$27:$I$27</definedName>
+    <definedName name="Trans_bands.columnindex" localSheetId="2" hidden="1">steelP!$B$34:$H$34</definedName>
     <definedName name="Trans_bands.columnindex.dirn" localSheetId="0" hidden="1">"column"</definedName>
+    <definedName name="Trans_bands.columnindex.dirn" localSheetId="2" hidden="1">"column"</definedName>
     <definedName name="Trans_bands.firstindex" localSheetId="0" hidden="1">"row"</definedName>
+    <definedName name="Trans_bands.firstindex" localSheetId="2" hidden="1">"row"</definedName>
     <definedName name="Trans_bands.rowindex" localSheetId="0" hidden="1">multi!$B$28:$B$30</definedName>
+    <definedName name="Trans_bands.rowindex" localSheetId="2" hidden="1">steelP!$A$35:$A$37</definedName>
     <definedName name="Trans_bands.rowindex.dirn" localSheetId="0" hidden="1">"row"</definedName>
+    <definedName name="Trans_bands.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
     <definedName name="Trans_coils" localSheetId="0">multi!$C$31:$I$33</definedName>
+    <definedName name="Trans_coils" localSheetId="2">steelP!$B$39:$H$41</definedName>
     <definedName name="Trans_coils.badindex" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="Trans_coils.badindex" localSheetId="2" hidden="1">1</definedName>
     <definedName name="Trans_coils.columnindex" localSheetId="0" hidden="1">multi!$C$27:$I$27</definedName>
+    <definedName name="Trans_coils.columnindex" localSheetId="2" hidden="1">steelP!$B$34:$H$34</definedName>
     <definedName name="Trans_coils.columnindex.dirn" localSheetId="0" hidden="1">"column"</definedName>
+    <definedName name="Trans_coils.columnindex.dirn" localSheetId="2" hidden="1">"column"</definedName>
     <definedName name="Trans_coils.firstindex" localSheetId="0" hidden="1">"row"</definedName>
+    <definedName name="Trans_coils.firstindex" localSheetId="2" hidden="1">"row"</definedName>
     <definedName name="Trans_coils.rowindex" localSheetId="0" hidden="1">multi!$B$31:$B$33</definedName>
+    <definedName name="Trans_coils.rowindex" localSheetId="2" hidden="1">steelP!$A$39:$A$41</definedName>
     <definedName name="Trans_coils.rowindex.dirn" localSheetId="0" hidden="1">"row"</definedName>
+    <definedName name="Trans_coils.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="trans_cost_bands" localSheetId="2">steelP!$B$22:$H$24</definedName>
+    <definedName name="trans_cost_bands.badindex" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="trans_cost_bands.columnindex" localSheetId="2" hidden="1">steelP!$B$17:$H$17</definedName>
+    <definedName name="trans_cost_bands.columnindex.dirn" localSheetId="2" hidden="1">"column"</definedName>
+    <definedName name="trans_cost_bands.firstindex" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="trans_cost_bands.rowindex" localSheetId="2" hidden="1">steelP!$A$22:$A$24</definedName>
+    <definedName name="trans_cost_bands.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="trans_cost_coils" localSheetId="2">steelP!$B$26:$H$28</definedName>
+    <definedName name="trans_cost_coils.badindex" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="trans_cost_coils.columnindex" localSheetId="2" hidden="1">steelP!$B$17:$H$17</definedName>
+    <definedName name="trans_cost_coils.columnindex.dirn" localSheetId="2" hidden="1">"column"</definedName>
+    <definedName name="trans_cost_coils.firstindex" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="trans_cost_coils.rowindex" localSheetId="2" hidden="1">steelP!$A$26:$A$28</definedName>
+    <definedName name="trans_cost_coils.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="trans_cost_plate" localSheetId="2">steelP!$B$30:$H$32</definedName>
+    <definedName name="trans_cost_plate.badindex" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="trans_cost_plate.columnindex" localSheetId="2" hidden="1">steelP!$B$17:$H$17</definedName>
+    <definedName name="trans_cost_plate.columnindex.dirn" localSheetId="2" hidden="1">"column"</definedName>
+    <definedName name="trans_cost_plate.firstindex" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="trans_cost_plate.rowindex" localSheetId="2" hidden="1">steelP!$A$30:$A$32</definedName>
+    <definedName name="trans_cost_plate.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
     <definedName name="Trans_plate" localSheetId="0">multi!$C$34:$I$36</definedName>
+    <definedName name="Trans_plate" localSheetId="2">steelP!$B$43:$H$45</definedName>
     <definedName name="Trans_plate.badindex" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="Trans_plate.badindex" localSheetId="2" hidden="1">1</definedName>
     <definedName name="Trans_plate.columnindex" localSheetId="0" hidden="1">multi!$C$27:$I$27</definedName>
+    <definedName name="Trans_plate.columnindex" localSheetId="2" hidden="1">steelP!$B$34:$H$34</definedName>
     <definedName name="Trans_plate.columnindex.dirn" localSheetId="0" hidden="1">"column"</definedName>
+    <definedName name="Trans_plate.columnindex.dirn" localSheetId="2" hidden="1">"column"</definedName>
     <definedName name="Trans_plate.firstindex" localSheetId="0" hidden="1">"row"</definedName>
+    <definedName name="Trans_plate.firstindex" localSheetId="2" hidden="1">"row"</definedName>
     <definedName name="Trans_plate.rowindex" localSheetId="0" hidden="1">multi!$B$34:$B$36</definedName>
+    <definedName name="Trans_plate.rowindex" localSheetId="2" hidden="1">steelP!$A$43:$A$45</definedName>
     <definedName name="Trans_plate.rowindex.dirn" localSheetId="0" hidden="1">"row"</definedName>
+    <definedName name="Trans_plate.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="49">
   <si>
     <t>cost</t>
   </si>
@@ -157,12 +305,87 @@
   <si>
     <t>Trans</t>
   </si>
+  <si>
+    <t>invcost</t>
+  </si>
+  <si>
+    <t>prodcost</t>
+  </si>
+  <si>
+    <t>inv0</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>avail</t>
+  </si>
+  <si>
+    <t>steelT</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>revenue</t>
+  </si>
+  <si>
+    <t>market</t>
+  </si>
+  <si>
+    <t>Make</t>
+  </si>
+  <si>
+    <t>Inv</t>
+  </si>
+  <si>
+    <t>Sell</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4 weeks</t>
+  </si>
+  <si>
+    <t>total_profit</t>
+  </si>
+  <si>
+    <t>CLEV</t>
+  </si>
+  <si>
+    <t>trans_cost_plate</t>
+  </si>
+  <si>
+    <t>trans_cost_coils</t>
+  </si>
+  <si>
+    <t>trans_cost_bands</t>
+  </si>
+  <si>
+    <t>make_cost</t>
+  </si>
+  <si>
+    <t>steelP.dat</t>
+  </si>
+  <si>
+    <t>Trans_bands</t>
+  </si>
+  <si>
+    <t>Trans_coils</t>
+  </si>
+  <si>
+    <t>Trans_plate</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>DUAL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +411,14 @@
     <font>
       <b/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -279,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -287,18 +518,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -318,6 +537,38 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2301,6 +2552,1253 @@
               <a:srgbClr val="FF0000"/>
             </a:solidFill>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>200026</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="270" name="TextBox 269"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3724276" y="4086225"/>
+          <a:ext cx="1352550" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Note</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> that Make and Sell are t in 1..T, but that Inv is </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> 0</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>..T.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="271" name="TextBox 270"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="114300" y="6010274"/>
+          <a:ext cx="4657725" cy="7924801"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ampl: model steelT.mod;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ampl: data steelT.dat;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ampl: solve;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>MINOS 5.51: optimal solution found.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>15 iterations, objective </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>515033</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ampl: show;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>parameters:       T   avail   inv0   invcost   </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>             market   prodcost   rate   revenue</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>set:           PROD</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>variables:     Inv   Make   Sell</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>constraints:   Balance   Init_Inv   Time</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>objective:     Total_Profit</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ampl: display Make;display Sell;    display Inv;  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Make</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> :=            </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Sell</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> :=          </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Inv</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> :=</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>                                    bands 0     10</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>bands 1   5990     bands 1   6000   bands 1      0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>bands 2   6000     bands 2   6000   bands 2      0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>bands 3   1400     bands 3   1400   bands 3      0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>bands 4   2000     bands 4   2000   bands 4      0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>                                    coils 0      0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>coils 1   1407     coils 1    307   coils 1   1100</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>coils 2   1400     coils 2   2500   coils 2      0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>coils 3   3500     coils 3   3500   coils 3      0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>coils 4   4200;    coils 4   4200;  coils 4      0;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>or</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> -----------------------------</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ampl: option </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>display_1col</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> 0;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ampl: display Make; display Inv; display Sell;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Make [*,*] (tr)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>:  bands  coils    :=</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>1   5990   1407</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>2   6000   1400</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>3   1400   3500</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>4   2000   4200;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Inv [*,*] (tr)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>: bands  coils    :=</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>0   10       0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>1    0    1100</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>2    0       0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>3    0       0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>4    0       0;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Sell [*,*] (tr)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>:  bands  coils    :=</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>1   6000    307</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>2   6000   2500</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>3   1400   3500</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>4   2000   4200;</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="273" name="Straight Arrow Connector 272"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2162175" y="5705475"/>
+          <a:ext cx="428625" cy="942975"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="123825" y="10887075"/>
+          <a:ext cx="4924425" cy="7410450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ampl: model steelP.mod;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ampl: data steelP.dat;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ampl: option solver CPLEX;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ampl: solve;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>CPLEX 12.7.0.0: optimal solution; objective 1392175</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>0 simplex iterations (0 in phase I)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ampl: option display_1col 5;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ampl: option omit_zero_rows 1, omit_zero_cols 1;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ampl: display Make;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Make</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> [*,*]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>:     bands  coils plate    :=</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>CLEV      0   1950     0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>GARY   1125   1750   300</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>PITT    775    500   500;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ampl: display Trans;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Trans</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> [CLEV,*,*]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>:   coils    :=</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>DET   750</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>LAF   500</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>LAN   400</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>STL    50</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>WIN   250</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> [GARY,*,*]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>:   bands coils plate    :=</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>FRE   225   850   100</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>LAF   250     0     0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>STL   650   900   200</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> [PITT,*,*]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>:   bands coils plate    :=</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>DET   300     0   100</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>FRA   300   500   100</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>LAF     0     0   250</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>LAN   100     0     0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>WIN    75     0    50;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ampl: display Time;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Time</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> [*] :=</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>CLEV  -1522.86</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>GARY  -3040;</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2598,8 +4096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2850,251 +4348,251 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="14">
         <v>30</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="14">
         <v>10</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="14">
         <v>8</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="14">
         <v>10</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="14">
         <v>11</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="14">
         <v>71</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="14">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17" t="s">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="14">
         <v>22</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="14">
         <v>7</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="14">
         <v>10</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="14">
         <v>7</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="14">
         <v>21</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="14">
         <v>82</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="14">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="14">
         <v>19</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="14">
         <v>11</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="14">
         <v>12</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="14">
         <v>10</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="14">
         <v>25</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H19" s="14">
         <v>83</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I19" s="14">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="11">
         <v>39</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="11">
         <v>14</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="11">
         <v>11</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="11">
         <v>14</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="11">
         <v>16</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20" s="11">
         <v>82</v>
       </c>
-      <c r="I20" s="15">
+      <c r="I20" s="11">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14" t="s">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="11">
         <v>27</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="11">
         <v>9</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="11">
         <v>12</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="11">
         <v>9</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="11">
         <v>26</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="11">
         <v>95</v>
       </c>
-      <c r="I21" s="15">
+      <c r="I21" s="11">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14" t="s">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="11">
         <v>24</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="11">
         <v>14</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="11">
         <v>17</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="11">
         <v>13</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="11">
         <v>28</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="11">
         <v>99</v>
       </c>
-      <c r="I22" s="15">
+      <c r="I22" s="11">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="8">
         <v>41</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="8">
         <v>15</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="8">
         <v>12</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="8">
         <v>16</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="8">
         <v>17</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="8">
         <v>86</v>
       </c>
-      <c r="I23" s="12">
+      <c r="I23" s="8">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="8">
         <v>29</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="8">
         <v>9</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="8">
         <v>13</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="8">
         <v>9</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="8">
         <v>28</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="8">
         <v>99</v>
       </c>
-      <c r="I24" s="12">
+      <c r="I24" s="8">
         <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11" t="s">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="8">
         <v>26</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="8">
         <v>14</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E25" s="8">
         <v>17</v>
       </c>
-      <c r="F25" s="12">
+      <c r="F25" s="8">
         <v>13</v>
       </c>
-      <c r="G25" s="12">
+      <c r="G25" s="8">
         <v>31</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H25" s="8">
         <v>104</v>
       </c>
-      <c r="I25" s="12">
+      <c r="I25" s="8">
         <v>20</v>
       </c>
     </row>
@@ -3125,269 +4623,269 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="18">
-        <v>0</v>
-      </c>
-      <c r="D28" s="18">
-        <v>0</v>
-      </c>
-      <c r="E28" s="18">
-        <v>0</v>
-      </c>
-      <c r="F28" s="18">
-        <v>0</v>
-      </c>
-      <c r="G28" s="18">
+      <c r="C28" s="14">
+        <v>0</v>
+      </c>
+      <c r="D28" s="14">
+        <v>0</v>
+      </c>
+      <c r="E28" s="14">
+        <v>0</v>
+      </c>
+      <c r="F28" s="14">
+        <v>0</v>
+      </c>
+      <c r="G28" s="14">
         <v>400</v>
       </c>
-      <c r="H28" s="18">
-        <v>0</v>
-      </c>
-      <c r="I28" s="18">
+      <c r="H28" s="14">
+        <v>0</v>
+      </c>
+      <c r="I28" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17" t="s">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="18">
+      <c r="C29" s="14">
         <v>275</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29" s="14">
         <v>100</v>
       </c>
-      <c r="E29" s="18">
-        <v>0</v>
-      </c>
-      <c r="F29" s="18">
+      <c r="E29" s="14">
+        <v>0</v>
+      </c>
+      <c r="F29" s="14">
         <v>75</v>
       </c>
-      <c r="G29" s="18">
+      <c r="G29" s="14">
         <v>250</v>
       </c>
-      <c r="H29" s="18">
-        <v>0</v>
-      </c>
-      <c r="I29" s="18">
+      <c r="H29" s="14">
+        <v>0</v>
+      </c>
+      <c r="I29" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17" t="s">
+      <c r="A30" s="13"/>
+      <c r="B30" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="18">
+      <c r="C30" s="14">
         <v>25</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D30" s="14">
         <v>200</v>
       </c>
-      <c r="E30" s="18">
+      <c r="E30" s="14">
         <v>100</v>
       </c>
-      <c r="F30" s="18">
-        <v>0</v>
-      </c>
-      <c r="G30" s="18">
-        <v>0</v>
-      </c>
-      <c r="H30" s="18">
+      <c r="F30" s="14">
+        <v>0</v>
+      </c>
+      <c r="G30" s="14">
+        <v>0</v>
+      </c>
+      <c r="H30" s="14">
         <v>225</v>
       </c>
-      <c r="I30" s="18">
+      <c r="I30" s="14">
         <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="15">
-        <v>0</v>
-      </c>
-      <c r="D31" s="15">
-        <v>0</v>
-      </c>
-      <c r="E31" s="15">
-        <v>0</v>
-      </c>
-      <c r="F31" s="15">
-        <v>0</v>
-      </c>
-      <c r="G31" s="15">
+      <c r="C31" s="11">
+        <v>0</v>
+      </c>
+      <c r="D31" s="11">
+        <v>0</v>
+      </c>
+      <c r="E31" s="11">
+        <v>0</v>
+      </c>
+      <c r="F31" s="11">
+        <v>0</v>
+      </c>
+      <c r="G31" s="11">
         <v>75</v>
       </c>
-      <c r="H31" s="15">
+      <c r="H31" s="11">
         <v>625</v>
       </c>
-      <c r="I31" s="15">
+      <c r="I31" s="11">
         <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14" t="s">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="15">
-        <v>0</v>
-      </c>
-      <c r="D32" s="15">
+      <c r="C32" s="11">
+        <v>0</v>
+      </c>
+      <c r="D32" s="11">
         <v>425</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="11">
         <v>400</v>
       </c>
-      <c r="F32" s="15">
+      <c r="F32" s="11">
         <v>250</v>
       </c>
-      <c r="G32" s="15">
+      <c r="G32" s="11">
         <v>250</v>
       </c>
-      <c r="H32" s="15">
+      <c r="H32" s="11">
         <v>50</v>
       </c>
-      <c r="I32" s="15">
+      <c r="I32" s="11">
         <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14" t="s">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="11">
         <v>500</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D33" s="11">
         <v>325</v>
       </c>
-      <c r="E33" s="15">
-        <v>0</v>
-      </c>
-      <c r="F33" s="15">
-        <v>0</v>
-      </c>
-      <c r="G33" s="15">
+      <c r="E33" s="11">
+        <v>0</v>
+      </c>
+      <c r="F33" s="11">
+        <v>0</v>
+      </c>
+      <c r="G33" s="11">
         <v>625</v>
       </c>
-      <c r="H33" s="15">
+      <c r="H33" s="11">
         <v>175</v>
       </c>
-      <c r="I33" s="15">
+      <c r="I33" s="11">
         <v>175</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="12">
-        <v>0</v>
-      </c>
-      <c r="D34" s="12">
-        <v>0</v>
-      </c>
-      <c r="E34" s="12">
-        <v>0</v>
-      </c>
-      <c r="F34" s="12">
-        <v>0</v>
-      </c>
-      <c r="G34" s="12">
+      <c r="C34" s="8">
+        <v>0</v>
+      </c>
+      <c r="D34" s="8">
+        <v>0</v>
+      </c>
+      <c r="E34" s="8">
+        <v>0</v>
+      </c>
+      <c r="F34" s="8">
+        <v>0</v>
+      </c>
+      <c r="G34" s="8">
         <v>150</v>
       </c>
-      <c r="H34" s="12">
-        <v>0</v>
-      </c>
-      <c r="I34" s="12">
+      <c r="H34" s="8">
+        <v>0</v>
+      </c>
+      <c r="I34" s="8">
         <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11" t="s">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="12">
-        <v>0</v>
-      </c>
-      <c r="D35" s="12">
+      <c r="C35" s="8">
+        <v>0</v>
+      </c>
+      <c r="D35" s="8">
         <v>100</v>
       </c>
-      <c r="E35" s="12">
-        <v>0</v>
-      </c>
-      <c r="F35" s="12">
+      <c r="E35" s="8">
+        <v>0</v>
+      </c>
+      <c r="F35" s="8">
         <v>50</v>
       </c>
-      <c r="G35" s="12">
+      <c r="G35" s="8">
         <v>50</v>
       </c>
-      <c r="H35" s="12">
+      <c r="H35" s="8">
         <v>100</v>
       </c>
-      <c r="I35" s="12">
+      <c r="I35" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11" t="s">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36" s="8">
         <v>100</v>
       </c>
-      <c r="D36" s="12">
-        <v>0</v>
-      </c>
-      <c r="E36" s="12">
-        <v>0</v>
-      </c>
-      <c r="F36" s="12">
-        <v>0</v>
-      </c>
-      <c r="G36" s="12">
-        <v>0</v>
-      </c>
-      <c r="H36" s="12">
-        <v>0</v>
-      </c>
-      <c r="I36" s="12">
+      <c r="D36" s="8">
+        <v>0</v>
+      </c>
+      <c r="E36" s="8">
+        <v>0</v>
+      </c>
+      <c r="F36" s="8">
+        <v>0</v>
+      </c>
+      <c r="G36" s="8">
+        <v>0</v>
+      </c>
+      <c r="H36" s="8">
+        <v>0</v>
+      </c>
+      <c r="I36" s="8">
         <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="6"/>
-      <c r="D38" s="19" t="s">
+      <c r="B38" s="17"/>
+      <c r="D38" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="D39" s="9">
+      <c r="B39" s="19"/>
+      <c r="D39" s="5">
         <v>199500</v>
       </c>
     </row>
@@ -3397,6 +4895,1412 @@
     <mergeCell ref="A39:B39"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2">
+        <v>200</v>
+      </c>
+      <c r="C3" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="2">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="2">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="20">
+        <v>1</v>
+      </c>
+      <c r="C9" s="20">
+        <v>2</v>
+      </c>
+      <c r="D9" s="20">
+        <v>3</v>
+      </c>
+      <c r="E9" s="20">
+        <v>4</v>
+      </c>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2">
+        <v>40</v>
+      </c>
+      <c r="D10" s="2">
+        <v>32</v>
+      </c>
+      <c r="E10" s="22">
+        <v>40</v>
+      </c>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2">
+        <v>26</v>
+      </c>
+      <c r="D13" s="2">
+        <v>27</v>
+      </c>
+      <c r="E13" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2">
+        <v>37</v>
+      </c>
+      <c r="E14" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2">
+        <v>6000</v>
+      </c>
+      <c r="C16" s="2">
+        <v>6000</v>
+      </c>
+      <c r="D16" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E16" s="2">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="2">
+        <v>4000</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2500</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3500</v>
+      </c>
+      <c r="E17" s="2">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="5">
+        <v>5990</v>
+      </c>
+      <c r="D20" s="5">
+        <v>6000</v>
+      </c>
+      <c r="E20" s="5">
+        <v>1399.9999999999998</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1999.9999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1407</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1400</v>
+      </c>
+      <c r="E21" s="5">
+        <v>3500</v>
+      </c>
+      <c r="F21" s="5">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="26">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="5">
+        <v>10</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1100</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="5">
+        <v>6000</v>
+      </c>
+      <c r="D26" s="5">
+        <v>6000</v>
+      </c>
+      <c r="E26" s="5">
+        <v>1399.9999999999998</v>
+      </c>
+      <c r="F26" s="5">
+        <v>1999.9999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="5">
+        <v>307</v>
+      </c>
+      <c r="D27" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E27" s="5">
+        <v>3500</v>
+      </c>
+      <c r="F27" s="5">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="17"/>
+      <c r="D29" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="19"/>
+      <c r="D30" s="25">
+        <v>515033</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2">
+        <v>200</v>
+      </c>
+      <c r="C9" s="2">
+        <v>190</v>
+      </c>
+      <c r="D9" s="2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>140</v>
+      </c>
+      <c r="C10" s="2">
+        <v>130</v>
+      </c>
+      <c r="D10" s="2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2">
+        <v>160</v>
+      </c>
+      <c r="C11" s="2">
+        <v>160</v>
+      </c>
+      <c r="D11" s="2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2">
+        <v>180</v>
+      </c>
+      <c r="C13" s="2">
+        <v>190</v>
+      </c>
+      <c r="D13" s="2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2">
+        <v>170</v>
+      </c>
+      <c r="C14" s="2">
+        <v>170</v>
+      </c>
+      <c r="D14" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2">
+        <v>180</v>
+      </c>
+      <c r="C15" s="2">
+        <v>185</v>
+      </c>
+      <c r="D15" s="2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2">
+        <v>300</v>
+      </c>
+      <c r="C18" s="2">
+        <v>300</v>
+      </c>
+      <c r="D18" s="2">
+        <v>100</v>
+      </c>
+      <c r="E18" s="2">
+        <v>75</v>
+      </c>
+      <c r="F18" s="2">
+        <v>650</v>
+      </c>
+      <c r="G18" s="2">
+        <v>225</v>
+      </c>
+      <c r="H18" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2">
+        <v>500</v>
+      </c>
+      <c r="C19" s="2">
+        <v>750</v>
+      </c>
+      <c r="D19" s="2">
+        <v>400</v>
+      </c>
+      <c r="E19" s="2">
+        <v>250</v>
+      </c>
+      <c r="F19" s="2">
+        <v>950</v>
+      </c>
+      <c r="G19" s="2">
+        <v>850</v>
+      </c>
+      <c r="H19" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2">
+        <v>100</v>
+      </c>
+      <c r="C20" s="2">
+        <v>100</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
+        <v>50</v>
+      </c>
+      <c r="F20" s="2">
+        <v>200</v>
+      </c>
+      <c r="G20" s="2">
+        <v>100</v>
+      </c>
+      <c r="H20" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="2">
+        <v>30</v>
+      </c>
+      <c r="C22" s="2">
+        <v>10</v>
+      </c>
+      <c r="D22" s="2">
+        <v>8</v>
+      </c>
+      <c r="E22" s="2">
+        <v>10</v>
+      </c>
+      <c r="F22" s="2">
+        <v>11</v>
+      </c>
+      <c r="G22" s="2">
+        <v>71</v>
+      </c>
+      <c r="H22" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="2">
+        <v>22</v>
+      </c>
+      <c r="C23" s="2">
+        <v>7</v>
+      </c>
+      <c r="D23" s="2">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2">
+        <v>7</v>
+      </c>
+      <c r="F23" s="2">
+        <v>21</v>
+      </c>
+      <c r="G23" s="2">
+        <v>82</v>
+      </c>
+      <c r="H23" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="2">
+        <v>19</v>
+      </c>
+      <c r="C24" s="2">
+        <v>11</v>
+      </c>
+      <c r="D24" s="2">
+        <v>12</v>
+      </c>
+      <c r="E24" s="2">
+        <v>10</v>
+      </c>
+      <c r="F24" s="2">
+        <v>25</v>
+      </c>
+      <c r="G24" s="2">
+        <v>83</v>
+      </c>
+      <c r="H24" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="2">
+        <v>39</v>
+      </c>
+      <c r="C26" s="2">
+        <v>14</v>
+      </c>
+      <c r="D26" s="2">
+        <v>11</v>
+      </c>
+      <c r="E26" s="2">
+        <v>14</v>
+      </c>
+      <c r="F26" s="2">
+        <v>16</v>
+      </c>
+      <c r="G26" s="2">
+        <v>82</v>
+      </c>
+      <c r="H26" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="2">
+        <v>27</v>
+      </c>
+      <c r="C27" s="2">
+        <v>9</v>
+      </c>
+      <c r="D27" s="2">
+        <v>12</v>
+      </c>
+      <c r="E27" s="2">
+        <v>9</v>
+      </c>
+      <c r="F27" s="2">
+        <v>26</v>
+      </c>
+      <c r="G27" s="2">
+        <v>95</v>
+      </c>
+      <c r="H27" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="2">
+        <v>24</v>
+      </c>
+      <c r="C28" s="2">
+        <v>14</v>
+      </c>
+      <c r="D28" s="2">
+        <v>17</v>
+      </c>
+      <c r="E28" s="2">
+        <v>13</v>
+      </c>
+      <c r="F28" s="2">
+        <v>28</v>
+      </c>
+      <c r="G28" s="2">
+        <v>99</v>
+      </c>
+      <c r="H28" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="2">
+        <v>41</v>
+      </c>
+      <c r="C30" s="2">
+        <v>15</v>
+      </c>
+      <c r="D30" s="2">
+        <v>12</v>
+      </c>
+      <c r="E30" s="2">
+        <v>16</v>
+      </c>
+      <c r="F30" s="2">
+        <v>17</v>
+      </c>
+      <c r="G30" s="2">
+        <v>86</v>
+      </c>
+      <c r="H30" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="2">
+        <v>29</v>
+      </c>
+      <c r="C31" s="2">
+        <v>9</v>
+      </c>
+      <c r="D31" s="2">
+        <v>13</v>
+      </c>
+      <c r="E31" s="2">
+        <v>9</v>
+      </c>
+      <c r="F31" s="2">
+        <v>28</v>
+      </c>
+      <c r="G31" s="2">
+        <v>99</v>
+      </c>
+      <c r="H31" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="2">
+        <v>26</v>
+      </c>
+      <c r="C32" s="2">
+        <v>14</v>
+      </c>
+      <c r="D32" s="2">
+        <v>17</v>
+      </c>
+      <c r="E32" s="2">
+        <v>13</v>
+      </c>
+      <c r="F32" s="2">
+        <v>31</v>
+      </c>
+      <c r="G32" s="2">
+        <v>104</v>
+      </c>
+      <c r="H32" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="5">
+        <v>0</v>
+      </c>
+      <c r="C35" s="5">
+        <v>0</v>
+      </c>
+      <c r="D35" s="5">
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <v>0</v>
+      </c>
+      <c r="F35" s="25">
+        <v>650</v>
+      </c>
+      <c r="G35" s="25">
+        <v>225</v>
+      </c>
+      <c r="H35" s="25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="5">
+        <v>0</v>
+      </c>
+      <c r="C36" s="5">
+        <v>0</v>
+      </c>
+      <c r="D36" s="5">
+        <v>0</v>
+      </c>
+      <c r="E36" s="5">
+        <v>0</v>
+      </c>
+      <c r="F36" s="5">
+        <v>0</v>
+      </c>
+      <c r="G36" s="5">
+        <v>0</v>
+      </c>
+      <c r="H36" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="25">
+        <v>300</v>
+      </c>
+      <c r="C37" s="25">
+        <v>300</v>
+      </c>
+      <c r="D37" s="25">
+        <v>100</v>
+      </c>
+      <c r="E37" s="25">
+        <v>75</v>
+      </c>
+      <c r="F37" s="5">
+        <v>0</v>
+      </c>
+      <c r="G37" s="5">
+        <v>0</v>
+      </c>
+      <c r="H37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="5">
+        <v>0</v>
+      </c>
+      <c r="C39" s="5">
+        <v>0</v>
+      </c>
+      <c r="D39" s="5">
+        <v>0</v>
+      </c>
+      <c r="E39" s="5">
+        <v>0</v>
+      </c>
+      <c r="F39" s="25">
+        <v>900</v>
+      </c>
+      <c r="G39" s="25">
+        <v>850</v>
+      </c>
+      <c r="H39" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="5">
+        <v>0</v>
+      </c>
+      <c r="C40" s="25">
+        <v>750</v>
+      </c>
+      <c r="D40" s="25">
+        <v>400</v>
+      </c>
+      <c r="E40" s="25">
+        <v>250</v>
+      </c>
+      <c r="F40" s="25">
+        <v>50</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0</v>
+      </c>
+      <c r="H40" s="25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="25">
+        <v>500</v>
+      </c>
+      <c r="C41" s="5">
+        <v>0</v>
+      </c>
+      <c r="D41" s="5">
+        <v>0</v>
+      </c>
+      <c r="E41" s="5">
+        <v>0</v>
+      </c>
+      <c r="F41" s="5">
+        <v>0</v>
+      </c>
+      <c r="G41" s="5">
+        <v>0</v>
+      </c>
+      <c r="H41" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="5">
+        <v>0</v>
+      </c>
+      <c r="C43" s="5">
+        <v>0</v>
+      </c>
+      <c r="D43" s="5">
+        <v>0</v>
+      </c>
+      <c r="E43" s="5">
+        <v>0</v>
+      </c>
+      <c r="F43" s="25">
+        <v>200</v>
+      </c>
+      <c r="G43" s="25">
+        <v>100</v>
+      </c>
+      <c r="H43" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="5">
+        <v>0</v>
+      </c>
+      <c r="C44" s="5">
+        <v>0</v>
+      </c>
+      <c r="D44" s="5">
+        <v>0</v>
+      </c>
+      <c r="E44" s="5">
+        <v>0</v>
+      </c>
+      <c r="F44" s="5">
+        <v>0</v>
+      </c>
+      <c r="G44" s="5">
+        <v>0</v>
+      </c>
+      <c r="H44" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="25">
+        <v>100</v>
+      </c>
+      <c r="C45" s="25">
+        <v>100</v>
+      </c>
+      <c r="D45" s="5">
+        <v>0</v>
+      </c>
+      <c r="E45" s="25">
+        <v>50</v>
+      </c>
+      <c r="F45" s="5">
+        <v>0</v>
+      </c>
+      <c r="G45" s="5">
+        <v>0</v>
+      </c>
+      <c r="H45" s="25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="5">
+        <v>1125</v>
+      </c>
+      <c r="C48" s="5">
+        <v>1750</v>
+      </c>
+      <c r="D48" s="5">
+        <v>300</v>
+      </c>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="5">
+        <v>0</v>
+      </c>
+      <c r="C49" s="5">
+        <v>1950</v>
+      </c>
+      <c r="D49" s="5">
+        <v>0</v>
+      </c>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="5">
+        <v>775</v>
+      </c>
+      <c r="C50" s="5">
+        <v>500</v>
+      </c>
+      <c r="D50" s="5">
+        <v>500</v>
+      </c>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" s="25">
+        <v>-2800</v>
+      </c>
+      <c r="C53" s="25">
+        <v>-1300</v>
+      </c>
+      <c r="D53" s="5">
+        <v>0</v>
+      </c>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" s="17"/>
+      <c r="D55" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" s="19"/>
+      <c r="D56" s="25">
+        <v>1392175</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -3418,12 +6322,12 @@
       sum {i in ORIG} supply[i,p] = sum {j in DEST} demand[j,p];
 param limit {ORIG,DEST} default 625 &gt;= 0;
 #Extra temporary variables for 2D&lt;=&gt;3D
-param cost_bands {ORIG,DEST}  &gt;= 0;  # shipment costs per unit
-param cost_coils {ORIG,DEST}  &gt;= 0;  # shipment costs per unit
-param cost_plate {ORIG,DEST}  &gt;= 0;  # shipment costs per unit
-param Trans_bands {ORIG,DEST} &gt;= 0;  # shipment costs per unit
-param Trans_coils {ORIG,DEST} &gt;= 0;  # shipment costs per unit
-param Trans_plate {ORIG,DEST} &gt;= 0;  # shipment costs per unit
+param cost_bands {ORIG,DEST}  &gt;= 0;  
+param cost_coils {ORIG,DEST}  &gt;= 0;  
+param cost_plate {ORIG,DEST}  &gt;= 0;  
+param Trans_bands {ORIG,DEST} &gt;= 0;  
+param Trans_coils {ORIG,DEST} &gt;= 0;  
+param Trans_plate {ORIG,DEST} &gt;= 0;  
 param cost {ORIG,DEST,PROD} &gt;= 0;  # shipment costs per unit
 var Trans {ORIG,DEST,PROD}  &gt;= 0;   # units to be shipped
 minimize Total_Cost:
@@ -3462,12 +6366,121 @@
   </FileText>
       <ParentWorksheetName>multi</ParentWorksheetName>
     </StoredFile>
+    <StoredFile>
+      <FileName>Untitled</FileName>
+      <LanguageName>AMPL</LanguageName>
+      <ModelPaneVisible>true</ModelPaneVisible>
+      <ModelSettings/>
+      <FileText>set PROD;       # products
+param T &gt; 0;    # number of weeks
+param rate {PROD} &gt; 0;          # tons per hour produced
+param inv0 {PROD} &gt;= 0;         # initial inventory
+param avail {1..T} &gt;= 0;        # hours available in week
+param market {PROD,1..T} &gt;= 0;  # limit on tons sold in week
+param prodcost {PROD} &gt;= 0;     # cost per ton produced
+param invcost {PROD} &gt;= 0;      # carrying cost/ton of inventory
+param revenue {PROD,1..T} &gt;= 0; # revenue per ton sold
+var Make {PROD,1..T} &gt;= 0;      # tons produced
+var Inv {PROD,0..T} &gt;= 0;       # tons inventoried
+var Sell {p in PROD, t in 1..T} &gt;= 0, &lt;= market[p,t]; # tons sold
+# Total revenue less costs in all weeks
+maximize total_profit:
+   sum {p in PROD, t in 1..T} (revenue[p,t]*Sell[p,t] -
+      prodcost[p]*Make[p,t] - invcost[p]*Inv[p,t]);
+# Total of hours used by all products
+# may not exceed hours available, in each week
+subject to time {t in 1..T}:
+   sum {p in PROD} (1/rate[p]) * Make[p,t] &lt;= avail[t];
+# Initial inventory must equal given value
+subject to initial {p in PROD}:  Inv[p,0] = inv0[p];
+# Tons produced and taken from inventory
+# must equal tons sold and put into inventory
+subject to balance {p in PROD, t in 1..T}:
+   Make[p,t] + Inv[p,t-1] = Sell[p,t] + Inv[p,t];
+#===================================================================
+# All lines below are optional if FixMinorErrors is checked
+#===================================================================
+# Get the data from the sheet
+data SheetData.dat;
+#option solver lpsolve;  #alternative solution, same cost
+option solver cbc;       #switch to COIN-CMDC solver
+solve;
+#solver info
+display solve_result &gt; Sheet;
+display total_profit &gt; Sheet;
+#solution info
+display Make &gt; Sheet;
+display Inv &gt; Sheet;
+display Sell &gt; Sheet;
+  </FileText>
+      <ParentWorksheetName>steelT</ParentWorksheetName>
+    </StoredFile>
+    <StoredFile>
+      <FileName>Untitled</FileName>
+      <LanguageName>AMPL</LanguageName>
+      <ModelPaneVisible>true</ModelPaneVisible>
+      <ModelSettings/>
+      <FileText>set ORIG;   # origins (steel mills)
+set DEST;   # destinations (factories)
+set PROD;   # products
+param rate {ORIG,PROD} &gt; 0;     # tons per hour at origins
+param avail {ORIG} &gt;= 0;        # hours available at origins
+param demand {DEST,PROD} &gt;= 0;  # tons required at destinations
+param make_cost {ORIG,PROD} &gt;= 0;        # manufacturing cost/ton
+param trans_cost {ORIG,DEST,PROD} &gt;= 0;  # shipping cost/ton
+var Make {ORIG,PROD} &gt;= 0;       # tons produced at origins
+var Trans {ORIG,DEST,PROD} &gt;= 0; # tons shipped
+#Extra temporary variables for 2D&lt;=&gt;3D
+param trans_cost_bands {ORIG,DEST}  &gt;= 0;  
+param trans_cost_coils {ORIG,DEST}  &gt;= 0;  
+param trans_cost_plate {ORIG,DEST}  &gt;= 0;  
+param Trans_bands {ORIG,DEST} &gt;= 0;  
+param Trans_coils {ORIG,DEST} &gt;= 0;  
+param Trans_plate {ORIG,DEST} &gt;= 0;  
+minimize Total_Cost:
+    sum {i in ORIG, p in PROD} make_cost[i,p] * Make[i,p] +
+        sum {i in ORIG, j in DEST, p in PROD}
+            trans_cost[i,j,p] * Trans[i,j,p];
+subject to Time {i in ORIG}:
+   sum {p in PROD} (1/rate[i,p]) * Make[i,p] &lt;= avail[i];
+subject to Supply {i in ORIG, p in PROD}:
+   sum {j in DEST} Trans[i,j,p] = Make[i,p];
+subject to Demand {j in DEST, p in PROD}:
+   sum {i in ORIG} Trans[i,j,p] = demand[j,p];
+#===================================================================
+# All lines below are optional if FixMinorErrors is checked
+#===================================================================
+# Get the data from the sheet
+data SheetData.dat;
+#move 2D SolverStudio DataItemEditor data to 3D AMPL variable
+let {i in ORIG, j in DEST} trans_cost[i,j,"bands"] := trans_cost_bands[i,j];
+let {i in ORIG, j in DEST} trans_cost[i,j,"coils"] := trans_cost_coils[i,j];
+let {i in ORIG, j in DEST} trans_cost[i,j,"plate"] := trans_cost_plate[i,j];
+#option solver lpsolve;  #alternative solution, same cost
+option solver cbc;       #switch to COIN-CMDC solver
+solve;
+#move 3D AMPL solution to the 2D SolverStudio solution variable
+let {i in ORIG, j in DEST} Trans_bands[i,j] := Trans[i,j,"bands"];
+let {i in ORIG, j in DEST} Trans_coils[i,j] := Trans[i,j,"coils"];
+let {i in ORIG, j in DEST} Trans_plate[i,j] := Trans[i,j,"plate"];
+#solution - pull the SolverStudio variables on to the sheet
+display Trans_bands &gt; Sheet;
+display Trans_coils &gt; Sheet;
+display Trans_plate &gt; Sheet;
+display Make &gt; Sheet;
+display Time &gt; Sheet;
+#solver info
+display solve_result &gt; Sheet;
+display Total_Cost &gt; Sheet;
+</FileText>
+      <ParentWorksheetName>steelP</ParentWorksheetName>
+    </StoredFile>
   </StoredFiles>
 </StoredFilesList>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7CE1CE0-CDB4-4B5B-9538-ABEAB88F8BC3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DBEE89-37CE-464D-8A23-173AD64532C7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://opensolver.org"/>

</xml_diff>